<commit_message>
updates after SF Referesh(Except EventExpenase)
</commit_message>
<xml_diff>
--- a/TestData/T1649_AdditionalClientsSubjectRequired.xlsx
+++ b/TestData/T1649_AdditionalClientsSubjectRequired.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sgoyal0427\source\repos\SalesForce_Project\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VKumar0427\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C451CDD0-780C-4F8E-AFB5-519416534319}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17250" windowHeight="4395"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AddOpportunity" sheetId="1" r:id="rId1"/>
@@ -20,14 +21,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -113,9 +106,6 @@
     <t>ClientInterest</t>
   </si>
   <si>
-    <t>Tec Alliance</t>
-  </si>
-  <si>
     <t>SFCAO User</t>
   </si>
   <si>
@@ -138,12 +128,15 @@
   </si>
   <si>
     <t>ABC</t>
+  </si>
+  <si>
+    <t>CB Alliance</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -181,11 +174,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -465,11 +456,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AI2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="AI2" sqref="AI2"/>
+    <sheetView tabSelected="1" topLeftCell="AK1" workbookViewId="0">
+      <selection activeCell="BM2" sqref="BM2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -487,6 +478,8 @@
     <col min="13" max="13" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.25">
@@ -536,11 +529,11 @@
         <v>24</v>
       </c>
       <c r="P1" s="1"/>
-      <c r="R1" s="2" t="s">
+      <c r="R1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>29</v>
       </c>
       <c r="AG1" s="1" t="s">
         <v>24</v>
@@ -553,11 +546,11 @@
       </c>
     </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>32</v>
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" t="s">
+        <v>31</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
@@ -587,31 +580,31 @@
         <v>16</v>
       </c>
       <c r="L2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M2" t="s">
         <v>19</v>
       </c>
       <c r="N2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="O2" t="s">
-        <v>26</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>30</v>
+        <v>34</v>
+      </c>
+      <c r="R2" t="s">
+        <v>29</v>
+      </c>
+      <c r="S2" t="s">
+        <v>29</v>
       </c>
       <c r="AG2" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="AH2" t="s">
         <v>10</v>
       </c>
       <c r="AI2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -621,7 +614,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -644,10 +637,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>